<commit_message>
les switch - plus basic aanpassing stage
</commit_message>
<xml_diff>
--- a/flyers/Mechelen_2020-21.xlsx
+++ b/flyers/Mechelen_2020-21.xlsx
@@ -310,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,16 +355,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -405,10 +401,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -580,15 +572,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:U134"/>
+  <dimension ref="B1:R134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="2.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="1.16"/>
@@ -1236,11 +1228,11 @@
         <v>17</v>
       </c>
       <c r="P19" s="7"/>
-      <c r="Q19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>16</v>
+      <c r="Q19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1268,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="M20" s="8"/>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="O20" s="7" t="n">
@@ -1303,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="M21" s="8"/>
-      <c r="N21" s="11" t="s">
+      <c r="N21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="O21" s="7" t="n">
@@ -1338,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="M22" s="8"/>
-      <c r="N22" s="11" t="s">
+      <c r="N22" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O22" s="7" t="n">
@@ -1373,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="M23" s="8"/>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="6" t="s">
         <v>13</v>
       </c>
       <c r="O23" s="7" t="n">
@@ -1408,17 +1400,17 @@
         <v>2</v>
       </c>
       <c r="M24" s="8"/>
-      <c r="N24" s="11" t="s">
+      <c r="N24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="O24" s="7" t="n">
         <v>22</v>
       </c>
       <c r="P24" s="7"/>
-      <c r="Q24" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R24" s="13" t="s">
+      <c r="Q24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R24" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1440,10 +1432,10 @@
         <v>23</v>
       </c>
       <c r="J25" s="9"/>
-      <c r="K25" s="14"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="9"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="11" t="s">
+      <c r="N25" s="6" t="s">
         <v>7</v>
       </c>
       <c r="O25" s="7" t="n">
@@ -1471,21 +1463,21 @@
         <v>24</v>
       </c>
       <c r="J26" s="9"/>
-      <c r="K26" s="14"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="9"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="11" t="s">
+      <c r="N26" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O26" s="7" t="n">
         <v>24</v>
       </c>
       <c r="P26" s="7"/>
-      <c r="Q26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R26" s="13" t="s">
-        <v>17</v>
+      <c r="Q26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1509,7 +1501,7 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="11" t="s">
+      <c r="N27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="O27" s="7" t="n">
@@ -1540,7 +1532,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="8"/>
-      <c r="N28" s="11" t="s">
+      <c r="N28" s="6" t="s">
         <v>8</v>
       </c>
       <c r="O28" s="7" t="n">
@@ -1571,7 +1563,7 @@
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="8"/>
-      <c r="N29" s="11" t="s">
+      <c r="N29" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O29" s="7" t="n">
@@ -1602,7 +1594,7 @@
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="8"/>
-      <c r="N30" s="11" t="s">
+      <c r="N30" s="6" t="s">
         <v>13</v>
       </c>
       <c r="O30" s="7" t="n">
@@ -1633,7 +1625,7 @@
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="8"/>
-      <c r="N31" s="11" t="s">
+      <c r="N31" s="6" t="s">
         <v>9</v>
       </c>
       <c r="O31" s="7" t="n">
@@ -1668,7 +1660,7 @@
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="8"/>
-      <c r="N32" s="11" t="s">
+      <c r="N32" s="6" t="s">
         <v>7</v>
       </c>
       <c r="O32" s="7" t="n">
@@ -1699,30 +1691,30 @@
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="8"/>
-      <c r="N33" s="11"/>
+      <c r="N33" s="6"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="4.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="17"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="17"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="16"/>
       <c r="M34" s="8"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="17"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="16"/>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="1"/>
@@ -1740,10 +1732,10 @@
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="18"/>
+      <c r="M35" s="17"/>
       <c r="N35" s="1"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="19" t="s">
+      <c r="P35" s="18" t="s">
         <v>20</v>
       </c>
       <c r="Q35" s="2"/>
@@ -1975,10 +1967,10 @@
         <v>6</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" s="13" t="s">
+      <c r="E42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G42" s="8"/>
@@ -2043,10 +2035,10 @@
         <v>8</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="E44" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F44" s="13" t="s">
+      <c r="E44" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="8"/>
@@ -2066,11 +2058,11 @@
       <c r="O44" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R44" s="13" t="s">
+      <c r="P44" s="19"/>
+      <c r="Q44" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R44" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2101,7 +2093,7 @@
       <c r="O45" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="P45" s="20"/>
+      <c r="P45" s="19"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
     </row>
@@ -2123,10 +2115,10 @@
         <v>10</v>
       </c>
       <c r="J46" s="7"/>
-      <c r="K46" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L46" s="13" t="s">
+      <c r="K46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M46" s="8"/>
@@ -2137,10 +2129,10 @@
         <v>10</v>
       </c>
       <c r="P46" s="7"/>
-      <c r="Q46" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R46" s="13" t="s">
+      <c r="Q46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R46" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2193,10 +2185,10 @@
         <v>12</v>
       </c>
       <c r="J48" s="7"/>
-      <c r="K48" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L48" s="13" t="s">
+      <c r="K48" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L48" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M48" s="8"/>
@@ -2241,7 +2233,7 @@
       <c r="O49" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="P49" s="21"/>
+      <c r="P49" s="20"/>
       <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
     </row>
@@ -2332,7 +2324,7 @@
       <c r="I52" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="J52" s="22"/>
+      <c r="J52" s="21"/>
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="M52" s="8"/>
@@ -2363,7 +2355,7 @@
       <c r="I53" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="J53" s="20"/>
+      <c r="J53" s="19"/>
       <c r="K53" s="10" t="s">
         <v>16</v>
       </c>
@@ -2425,7 +2417,7 @@
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
-      <c r="F55" s="23"/>
+      <c r="F55" s="22"/>
       <c r="G55" s="8"/>
       <c r="H55" s="6" t="s">
         <v>10</v>
@@ -2459,10 +2451,10 @@
         <v>20</v>
       </c>
       <c r="D56" s="7"/>
-      <c r="E56" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F56" s="13" t="s">
+      <c r="E56" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G56" s="8"/>
@@ -2527,10 +2519,10 @@
         <v>22</v>
       </c>
       <c r="D58" s="7"/>
-      <c r="E58" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F58" s="13" t="s">
+      <c r="E58" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G58" s="8"/>
@@ -2588,9 +2580,6 @@
         <v>22</v>
       </c>
       <c r="R59" s="9"/>
-      <c r="S59" s="24"/>
-      <c r="T59" s="24"/>
-      <c r="U59" s="24"/>
     </row>
     <row r="60" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="6" t="s">
@@ -2610,10 +2599,10 @@
         <v>24</v>
       </c>
       <c r="J60" s="7"/>
-      <c r="K60" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="13" t="s">
+      <c r="K60" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M60" s="8"/>
@@ -2628,9 +2617,6 @@
         <v>22</v>
       </c>
       <c r="R60" s="9"/>
-      <c r="S60" s="24"/>
-      <c r="T60" s="24"/>
-      <c r="U60" s="24"/>
     </row>
     <row r="61" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="6" t="s">
@@ -2664,9 +2650,6 @@
         <v>22</v>
       </c>
       <c r="R61" s="9"/>
-      <c r="S61" s="24"/>
-      <c r="T61" s="24"/>
-      <c r="U61" s="24"/>
     </row>
     <row r="62" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="6" t="s">
@@ -2686,10 +2669,10 @@
         <v>26</v>
       </c>
       <c r="J62" s="7"/>
-      <c r="K62" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L62" s="13" t="s">
+      <c r="K62" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L62" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M62" s="8"/>
@@ -2702,9 +2685,6 @@
       <c r="P62" s="9"/>
       <c r="Q62" s="9"/>
       <c r="R62" s="9"/>
-      <c r="S62" s="24"/>
-      <c r="T62" s="24"/>
-      <c r="U62" s="24"/>
     </row>
     <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="6" t="s">
@@ -2740,9 +2720,6 @@
       <c r="P63" s="9"/>
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
-      <c r="S63" s="24"/>
-      <c r="T63" s="24"/>
-      <c r="U63" s="24"/>
     </row>
     <row r="64" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="6" t="s">
@@ -2776,9 +2753,6 @@
         <v>22</v>
       </c>
       <c r="R64" s="9"/>
-      <c r="S64" s="24"/>
-      <c r="T64" s="24"/>
-      <c r="U64" s="24"/>
     </row>
     <row r="65" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="6" t="s">
@@ -2816,9 +2790,6 @@
         <v>22</v>
       </c>
       <c r="R65" s="9"/>
-      <c r="S65" s="24"/>
-      <c r="T65" s="24"/>
-      <c r="U65" s="24"/>
     </row>
     <row r="66" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="6" t="s">
@@ -2852,9 +2823,6 @@
         <v>22</v>
       </c>
       <c r="R66" s="9"/>
-      <c r="S66" s="24"/>
-      <c r="T66" s="24"/>
-      <c r="U66" s="24"/>
     </row>
     <row r="67" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="6" t="s">
@@ -2884,78 +2852,72 @@
         <v>22</v>
       </c>
       <c r="R67" s="9"/>
-      <c r="S67" s="24"/>
-      <c r="T67" s="24"/>
-      <c r="U67" s="24"/>
     </row>
     <row r="68" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="1"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="25" t="s">
+      <c r="D68" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="26"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="28"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="26"/>
-      <c r="J68" s="25" t="s">
+      <c r="E68" s="24"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="24"/>
+      <c r="J68" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="K68" s="26"/>
-      <c r="L68" s="27"/>
-      <c r="M68" s="28"/>
-      <c r="N68" s="29"/>
-      <c r="O68" s="26"/>
-      <c r="P68" s="25" t="s">
+      <c r="K68" s="24"/>
+      <c r="L68" s="25"/>
+      <c r="M68" s="26"/>
+      <c r="N68" s="27"/>
+      <c r="O68" s="24"/>
+      <c r="P68" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="Q68" s="26"/>
-      <c r="R68" s="27"/>
-      <c r="S68" s="24"/>
-      <c r="T68" s="24"/>
-      <c r="U68" s="24"/>
+      <c r="Q68" s="24"/>
+      <c r="R68" s="25"/>
     </row>
     <row r="69" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C69" s="7"/>
-      <c r="D69" s="30" t="s">
+      <c r="D69" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F69" s="30" t="s">
+      <c r="F69" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G69" s="28"/>
-      <c r="H69" s="31" t="s">
+      <c r="G69" s="26"/>
+      <c r="H69" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30" t="s">
+      <c r="I69" s="28"/>
+      <c r="J69" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K69" s="30" t="s">
+      <c r="K69" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="L69" s="30" t="s">
+      <c r="L69" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M69" s="28"/>
-      <c r="N69" s="31" t="s">
+      <c r="M69" s="26"/>
+      <c r="N69" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="O69" s="30"/>
-      <c r="P69" s="30" t="s">
+      <c r="O69" s="28"/>
+      <c r="P69" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Q69" s="30" t="s">
+      <c r="Q69" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="R69" s="30" t="s">
+      <c r="R69" s="28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2966,31 +2928,31 @@
       <c r="C70" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32" t="s">
+      <c r="D70" s="30"/>
+      <c r="E70" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F70" s="32"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" s="30" t="n">
+      <c r="F70" s="30"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="J70" s="34"/>
-      <c r="K70" s="30"/>
-      <c r="L70" s="30"/>
-      <c r="M70" s="28"/>
-      <c r="N70" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O70" s="30" t="n">
+      <c r="J70" s="32"/>
+      <c r="K70" s="28"/>
+      <c r="L70" s="28"/>
+      <c r="M70" s="26"/>
+      <c r="N70" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O70" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="P70" s="30"/>
-      <c r="Q70" s="30"/>
-      <c r="R70" s="30"/>
+      <c r="P70" s="28"/>
+      <c r="Q70" s="28"/>
+      <c r="R70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="6" t="s">
@@ -2999,31 +2961,31 @@
       <c r="C71" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I71" s="30" t="n">
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I71" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="J71" s="30"/>
-      <c r="K71" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L71" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M71" s="28"/>
-      <c r="N71" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O71" s="30" t="n">
+      <c r="J71" s="28"/>
+      <c r="K71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M71" s="26"/>
+      <c r="N71" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O71" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="P71" s="30"/>
+      <c r="P71" s="28"/>
       <c r="Q71" s="10" t="s">
         <v>16</v>
       </c>
@@ -3038,27 +3000,27 @@
       <c r="C72" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I72" s="30" t="n">
+      <c r="D72" s="30"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="J72" s="30"/>
+      <c r="J72" s="28"/>
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
-      <c r="M72" s="28"/>
-      <c r="N72" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O72" s="30" t="n">
+      <c r="M72" s="26"/>
+      <c r="N72" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O72" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="P72" s="30"/>
+      <c r="P72" s="28"/>
       <c r="Q72" s="7"/>
       <c r="R72" s="7"/>
     </row>
@@ -3069,31 +3031,31 @@
       <c r="C73" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I73" s="30" t="n">
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I73" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="J73" s="30"/>
-      <c r="K73" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L73" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M73" s="28"/>
-      <c r="N73" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O73" s="30" t="n">
+      <c r="J73" s="28"/>
+      <c r="K73" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L73" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M73" s="26"/>
+      <c r="N73" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O73" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="P73" s="30"/>
+      <c r="P73" s="28"/>
       <c r="Q73" s="10" t="s">
         <v>16</v>
       </c>
@@ -3108,31 +3070,31 @@
       <c r="C74" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F74" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G74" s="28"/>
-      <c r="H74" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74" s="30" t="n">
+      <c r="D74" s="28"/>
+      <c r="E74" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G74" s="26"/>
+      <c r="H74" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I74" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="J74" s="30"/>
-      <c r="K74" s="30"/>
-      <c r="L74" s="30"/>
-      <c r="M74" s="28"/>
-      <c r="N74" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O74" s="30" t="n">
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O74" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="P74" s="34"/>
+      <c r="P74" s="32"/>
       <c r="Q74" s="7"/>
       <c r="R74" s="7"/>
     </row>
@@ -3143,29 +3105,29 @@
       <c r="C75" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="D75" s="30"/>
+      <c r="D75" s="28"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I75" s="30" t="n">
+      <c r="G75" s="26"/>
+      <c r="H75" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I75" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="J75" s="32"/>
+      <c r="J75" s="30"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
-      <c r="M75" s="28"/>
-      <c r="N75" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O75" s="30" t="n">
+      <c r="M75" s="26"/>
+      <c r="N75" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O75" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="P75" s="35"/>
-      <c r="Q75" s="32"/>
-      <c r="R75" s="32"/>
+      <c r="P75" s="33"/>
+      <c r="Q75" s="30"/>
+      <c r="R75" s="30"/>
     </row>
     <row r="76" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="6" t="s">
@@ -3174,33 +3136,33 @@
       <c r="C76" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="D76" s="30"/>
-      <c r="E76" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F76" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G76" s="28"/>
-      <c r="H76" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I76" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
-      <c r="L76" s="32"/>
-      <c r="M76" s="28"/>
-      <c r="N76" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O76" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="P76" s="32"/>
-      <c r="Q76" s="32"/>
-      <c r="R76" s="32"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G76" s="26"/>
+      <c r="H76" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="J76" s="30"/>
+      <c r="K76" s="30"/>
+      <c r="L76" s="30"/>
+      <c r="M76" s="26"/>
+      <c r="N76" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O76" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="P76" s="30"/>
+      <c r="Q76" s="30"/>
+      <c r="R76" s="30"/>
     </row>
     <row r="77" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="6" t="s">
@@ -3209,29 +3171,29 @@
       <c r="C77" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
-      <c r="G77" s="28"/>
-      <c r="H77" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I77" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="J77" s="30"/>
-      <c r="K77" s="30"/>
-      <c r="L77" s="30"/>
-      <c r="M77" s="28"/>
-      <c r="N77" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O77" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="P77" s="30"/>
-      <c r="Q77" s="30"/>
-      <c r="R77" s="30"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="26"/>
+      <c r="H77" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="J77" s="28"/>
+      <c r="K77" s="28"/>
+      <c r="L77" s="28"/>
+      <c r="M77" s="26"/>
+      <c r="N77" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O77" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="P77" s="28"/>
+      <c r="Q77" s="28"/>
+      <c r="R77" s="28"/>
     </row>
     <row r="78" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="6" t="s">
@@ -3240,35 +3202,35 @@
       <c r="C78" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="D78" s="32"/>
+      <c r="D78" s="30"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
-      <c r="G78" s="28"/>
-      <c r="H78" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I78" s="30" t="n">
-        <v>9</v>
-      </c>
-      <c r="J78" s="30"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I78" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="J78" s="28"/>
       <c r="K78" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L78" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M78" s="28"/>
-      <c r="N78" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O78" s="30" t="n">
-        <v>9</v>
-      </c>
-      <c r="P78" s="30"/>
-      <c r="Q78" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R78" s="13" t="s">
+      <c r="M78" s="26"/>
+      <c r="N78" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O78" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="P78" s="28"/>
+      <c r="Q78" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R78" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3279,27 +3241,27 @@
       <c r="C79" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="D79" s="32"/>
-      <c r="E79" s="32"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="28"/>
-      <c r="H79" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I79" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="J79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I79" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="J79" s="28"/>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
-      <c r="M79" s="28"/>
-      <c r="N79" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O79" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="P79" s="30"/>
+      <c r="M79" s="26"/>
+      <c r="N79" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O79" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="P79" s="28"/>
       <c r="Q79" s="7"/>
       <c r="R79" s="7"/>
     </row>
@@ -3310,35 +3272,35 @@
       <c r="C80" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
-      <c r="G80" s="28"/>
-      <c r="H80" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I80" s="30" t="n">
-        <v>11</v>
-      </c>
-      <c r="J80" s="34"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I80" s="28" t="n">
+        <v>11</v>
+      </c>
+      <c r="J80" s="32"/>
       <c r="K80" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L80" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="M80" s="28"/>
-      <c r="N80" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O80" s="30" t="n">
-        <v>11</v>
-      </c>
-      <c r="P80" s="34"/>
-      <c r="Q80" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R80" s="13" t="s">
+      <c r="M80" s="26"/>
+      <c r="N80" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O80" s="28" t="n">
+        <v>11</v>
+      </c>
+      <c r="P80" s="32"/>
+      <c r="Q80" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R80" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3349,31 +3311,31 @@
       <c r="C81" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="D81" s="30"/>
+      <c r="D81" s="28"/>
       <c r="E81" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F81" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G81" s="28"/>
-      <c r="H81" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I81" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="J81" s="34"/>
-      <c r="K81" s="30"/>
-      <c r="L81" s="30"/>
-      <c r="M81" s="28"/>
-      <c r="N81" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O81" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="P81" s="34"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I81" s="28" t="n">
+        <v>12</v>
+      </c>
+      <c r="J81" s="32"/>
+      <c r="K81" s="28"/>
+      <c r="L81" s="28"/>
+      <c r="M81" s="26"/>
+      <c r="N81" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O81" s="28" t="n">
+        <v>12</v>
+      </c>
+      <c r="P81" s="32"/>
       <c r="Q81" s="7"/>
       <c r="R81" s="7"/>
     </row>
@@ -3384,29 +3346,29 @@
       <c r="C82" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
-      <c r="F82" s="30"/>
-      <c r="G82" s="28"/>
-      <c r="H82" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I82" s="30" t="n">
-        <v>13</v>
-      </c>
-      <c r="J82" s="35"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="J82" s="33"/>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
-      <c r="M82" s="28"/>
-      <c r="N82" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O82" s="30" t="n">
-        <v>13</v>
-      </c>
-      <c r="P82" s="35"/>
-      <c r="Q82" s="32"/>
-      <c r="R82" s="32"/>
+      <c r="M82" s="26"/>
+      <c r="N82" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O82" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="P82" s="33"/>
+      <c r="Q82" s="30"/>
+      <c r="R82" s="30"/>
     </row>
     <row r="83" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="6" t="s">
@@ -3415,33 +3377,33 @@
       <c r="C83" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="D83" s="34"/>
+      <c r="D83" s="32"/>
       <c r="E83" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G83" s="28"/>
-      <c r="H83" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I83" s="30" t="n">
+      <c r="G83" s="26"/>
+      <c r="H83" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I83" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="J83" s="35"/>
-      <c r="K83" s="32"/>
-      <c r="L83" s="32"/>
-      <c r="M83" s="28"/>
-      <c r="N83" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O83" s="30" t="n">
+      <c r="J83" s="33"/>
+      <c r="K83" s="30"/>
+      <c r="L83" s="30"/>
+      <c r="M83" s="26"/>
+      <c r="N83" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O83" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="P83" s="35"/>
-      <c r="Q83" s="32"/>
-      <c r="R83" s="32"/>
+      <c r="P83" s="33"/>
+      <c r="Q83" s="30"/>
+      <c r="R83" s="30"/>
     </row>
     <row r="84" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="6" t="s">
@@ -3450,31 +3412,31 @@
       <c r="C84" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="D84" s="34"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="30"/>
-      <c r="G84" s="28"/>
-      <c r="H84" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I84" s="30" t="n">
+      <c r="D84" s="32"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="26"/>
+      <c r="H84" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="J84" s="32"/>
-      <c r="K84" s="32" t="s">
+      <c r="J84" s="30"/>
+      <c r="K84" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L84" s="32"/>
-      <c r="M84" s="28"/>
-      <c r="N84" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O84" s="30" t="n">
+      <c r="L84" s="30"/>
+      <c r="M84" s="26"/>
+      <c r="N84" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O84" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="P84" s="34"/>
-      <c r="Q84" s="30"/>
-      <c r="R84" s="30"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="28"/>
+      <c r="R84" s="28"/>
     </row>
     <row r="85" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="6" t="s">
@@ -3483,29 +3445,29 @@
       <c r="C85" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="D85" s="35"/>
+      <c r="D85" s="33"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
-      <c r="G85" s="28"/>
-      <c r="H85" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I85" s="30" t="n">
-        <v>16</v>
-      </c>
-      <c r="J85" s="35"/>
-      <c r="K85" s="32" t="s">
+      <c r="G85" s="26"/>
+      <c r="H85" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I85" s="28" t="n">
+        <v>16</v>
+      </c>
+      <c r="J85" s="33"/>
+      <c r="K85" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L85" s="32"/>
-      <c r="M85" s="28"/>
-      <c r="N85" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O85" s="30" t="n">
-        <v>16</v>
-      </c>
-      <c r="P85" s="34"/>
+      <c r="L85" s="30"/>
+      <c r="M85" s="26"/>
+      <c r="N85" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O85" s="28" t="n">
+        <v>16</v>
+      </c>
+      <c r="P85" s="32"/>
       <c r="Q85" s="10" t="s">
         <v>16</v>
       </c>
@@ -3520,29 +3482,29 @@
       <c r="C86" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="D86" s="35"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I86" s="30" t="n">
-        <v>17</v>
-      </c>
-      <c r="J86" s="35"/>
-      <c r="K86" s="32" t="s">
+      <c r="D86" s="33"/>
+      <c r="E86" s="30"/>
+      <c r="F86" s="30"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="28" t="n">
+        <v>17</v>
+      </c>
+      <c r="J86" s="33"/>
+      <c r="K86" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L86" s="32"/>
-      <c r="M86" s="28"/>
-      <c r="N86" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O86" s="30" t="n">
-        <v>17</v>
-      </c>
-      <c r="P86" s="34"/>
+      <c r="L86" s="30"/>
+      <c r="M86" s="26"/>
+      <c r="N86" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O86" s="28" t="n">
+        <v>17</v>
+      </c>
+      <c r="P86" s="32"/>
       <c r="Q86" s="7"/>
       <c r="R86" s="7"/>
     </row>
@@ -3553,29 +3515,29 @@
       <c r="C87" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D87" s="34"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="30"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I87" s="30" t="n">
+      <c r="D87" s="32"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I87" s="28" t="n">
         <v>18</v>
       </c>
-      <c r="J87" s="35"/>
+      <c r="J87" s="33"/>
       <c r="K87" s="9" t="s">
         <v>21</v>
       </c>
       <c r="L87" s="9"/>
-      <c r="M87" s="28"/>
-      <c r="N87" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O87" s="30" t="n">
+      <c r="M87" s="26"/>
+      <c r="N87" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O87" s="28" t="n">
         <v>18</v>
       </c>
-      <c r="P87" s="34"/>
+      <c r="P87" s="32"/>
       <c r="Q87" s="10" t="s">
         <v>16</v>
       </c>
@@ -3590,33 +3552,33 @@
       <c r="C88" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="D88" s="30"/>
-      <c r="E88" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F88" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G88" s="28"/>
-      <c r="H88" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I88" s="30" t="n">
+      <c r="D88" s="28"/>
+      <c r="E88" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G88" s="26"/>
+      <c r="H88" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I88" s="28" t="n">
         <v>19</v>
       </c>
-      <c r="J88" s="35"/>
-      <c r="K88" s="32" t="s">
+      <c r="J88" s="33"/>
+      <c r="K88" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L88" s="32"/>
-      <c r="M88" s="28"/>
-      <c r="N88" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O88" s="30" t="n">
+      <c r="L88" s="30"/>
+      <c r="M88" s="26"/>
+      <c r="N88" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O88" s="28" t="n">
         <v>19</v>
       </c>
-      <c r="P88" s="34"/>
+      <c r="P88" s="32"/>
       <c r="Q88" s="7"/>
       <c r="R88" s="7"/>
     </row>
@@ -3627,29 +3589,29 @@
       <c r="C89" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="D89" s="30"/>
+      <c r="D89" s="28"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
-      <c r="G89" s="28"/>
-      <c r="H89" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I89" s="30" t="n">
+      <c r="G89" s="26"/>
+      <c r="H89" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I89" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="J89" s="35"/>
+      <c r="J89" s="33"/>
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
-      <c r="M89" s="28"/>
-      <c r="N89" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O89" s="30" t="n">
+      <c r="M89" s="26"/>
+      <c r="N89" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O89" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="P89" s="35"/>
-      <c r="Q89" s="32"/>
-      <c r="R89" s="32"/>
+      <c r="P89" s="33"/>
+      <c r="Q89" s="30"/>
+      <c r="R89" s="30"/>
     </row>
     <row r="90" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="6" t="s">
@@ -3658,33 +3620,33 @@
       <c r="C90" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="D90" s="30"/>
-      <c r="E90" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F90" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G90" s="28"/>
-      <c r="H90" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I90" s="30" t="n">
+      <c r="D90" s="28"/>
+      <c r="E90" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G90" s="26"/>
+      <c r="H90" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I90" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="J90" s="35"/>
-      <c r="K90" s="32"/>
-      <c r="L90" s="32"/>
-      <c r="M90" s="28"/>
-      <c r="N90" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O90" s="30" t="n">
+      <c r="J90" s="33"/>
+      <c r="K90" s="30"/>
+      <c r="L90" s="30"/>
+      <c r="M90" s="26"/>
+      <c r="N90" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O90" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="P90" s="35"/>
-      <c r="Q90" s="32"/>
-      <c r="R90" s="32"/>
+      <c r="P90" s="33"/>
+      <c r="Q90" s="30"/>
+      <c r="R90" s="30"/>
     </row>
     <row r="91" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="6" t="s">
@@ -3693,29 +3655,29 @@
       <c r="C91" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="30"/>
-      <c r="G91" s="28"/>
-      <c r="H91" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I91" s="30" t="n">
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="26"/>
+      <c r="H91" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I91" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="J91" s="34"/>
-      <c r="K91" s="30"/>
-      <c r="L91" s="30"/>
-      <c r="M91" s="28"/>
-      <c r="N91" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O91" s="30" t="n">
+      <c r="J91" s="32"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="28"/>
+      <c r="M91" s="26"/>
+      <c r="N91" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O91" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="P91" s="34"/>
-      <c r="Q91" s="30"/>
-      <c r="R91" s="30"/>
+      <c r="P91" s="32"/>
+      <c r="Q91" s="28"/>
+      <c r="R91" s="28"/>
     </row>
     <row r="92" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="6" t="s">
@@ -3724,35 +3686,35 @@
       <c r="C92" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="D92" s="32"/>
+      <c r="D92" s="30"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
-      <c r="G92" s="28"/>
-      <c r="H92" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I92" s="30" t="n">
+      <c r="G92" s="26"/>
+      <c r="H92" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I92" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="J92" s="30"/>
-      <c r="K92" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L92" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M92" s="28"/>
-      <c r="N92" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O92" s="30" t="n">
+      <c r="J92" s="28"/>
+      <c r="K92" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L92" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M92" s="26"/>
+      <c r="N92" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O92" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="P92" s="34"/>
-      <c r="Q92" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R92" s="13" t="s">
+      <c r="P92" s="32"/>
+      <c r="Q92" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R92" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3763,27 +3725,27 @@
       <c r="C93" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="28"/>
-      <c r="H93" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I93" s="30" t="n">
+      <c r="D93" s="30"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="J93" s="30"/>
+      <c r="J93" s="28"/>
       <c r="K93" s="7"/>
       <c r="L93" s="7"/>
-      <c r="M93" s="28"/>
-      <c r="N93" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O93" s="30" t="n">
+      <c r="M93" s="26"/>
+      <c r="N93" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O93" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="P93" s="34"/>
+      <c r="P93" s="32"/>
       <c r="Q93" s="7"/>
       <c r="R93" s="7"/>
     </row>
@@ -3794,35 +3756,35 @@
       <c r="C94" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I94" s="30" t="n">
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I94" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="J94" s="30"/>
-      <c r="K94" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L94" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M94" s="28"/>
-      <c r="N94" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O94" s="30" t="n">
+      <c r="J94" s="28"/>
+      <c r="K94" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L94" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M94" s="26"/>
+      <c r="N94" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O94" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="P94" s="30"/>
-      <c r="Q94" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R94" s="13" t="s">
+      <c r="P94" s="28"/>
+      <c r="Q94" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R94" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3833,31 +3795,31 @@
       <c r="C95" s="7" t="n">
         <v>26</v>
       </c>
-      <c r="D95" s="30"/>
+      <c r="D95" s="28"/>
       <c r="E95" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F95" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G95" s="28"/>
-      <c r="H95" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I95" s="30" t="n">
+      <c r="G95" s="26"/>
+      <c r="H95" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I95" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="J95" s="30"/>
-      <c r="K95" s="30"/>
-      <c r="L95" s="30"/>
-      <c r="M95" s="28"/>
-      <c r="N95" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O95" s="30" t="n">
+      <c r="J95" s="28"/>
+      <c r="K95" s="28"/>
+      <c r="L95" s="28"/>
+      <c r="M95" s="26"/>
+      <c r="N95" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O95" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="P95" s="30"/>
+      <c r="P95" s="28"/>
       <c r="Q95" s="7"/>
       <c r="R95" s="7"/>
     </row>
@@ -3868,29 +3830,29 @@
       <c r="C96" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="D96" s="30"/>
+      <c r="D96" s="28"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I96" s="30" t="n">
+      <c r="G96" s="26"/>
+      <c r="H96" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="J96" s="32"/>
-      <c r="K96" s="32"/>
-      <c r="L96" s="32"/>
-      <c r="M96" s="28"/>
-      <c r="N96" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O96" s="30" t="n">
+      <c r="J96" s="30"/>
+      <c r="K96" s="30"/>
+      <c r="L96" s="30"/>
+      <c r="M96" s="26"/>
+      <c r="N96" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O96" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="P96" s="32"/>
-      <c r="Q96" s="32"/>
-      <c r="R96" s="32"/>
+      <c r="P96" s="30"/>
+      <c r="Q96" s="30"/>
+      <c r="R96" s="30"/>
     </row>
     <row r="97" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="6" t="s">
@@ -3899,33 +3861,33 @@
       <c r="C97" s="7" t="n">
         <v>28</v>
       </c>
-      <c r="D97" s="34"/>
+      <c r="D97" s="32"/>
       <c r="E97" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G97" s="28"/>
-      <c r="H97" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I97" s="30" t="n">
+      <c r="G97" s="26"/>
+      <c r="H97" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I97" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="J97" s="32"/>
-      <c r="K97" s="32"/>
-      <c r="L97" s="32"/>
-      <c r="M97" s="28"/>
-      <c r="N97" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O97" s="30" t="n">
+      <c r="J97" s="30"/>
+      <c r="K97" s="30"/>
+      <c r="L97" s="30"/>
+      <c r="M97" s="26"/>
+      <c r="N97" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O97" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="P97" s="32"/>
-      <c r="Q97" s="32"/>
-      <c r="R97" s="32"/>
+      <c r="P97" s="30"/>
+      <c r="Q97" s="30"/>
+      <c r="R97" s="30"/>
     </row>
     <row r="98" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="6" t="s">
@@ -3934,25 +3896,25 @@
       <c r="C98" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="D98" s="34"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="33"/>
-      <c r="I98" s="36"/>
-      <c r="J98" s="30"/>
-      <c r="K98" s="30"/>
-      <c r="L98" s="30"/>
-      <c r="M98" s="28"/>
-      <c r="N98" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O98" s="30" t="n">
+      <c r="D98" s="32"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="31"/>
+      <c r="I98" s="34"/>
+      <c r="J98" s="28"/>
+      <c r="K98" s="28"/>
+      <c r="L98" s="28"/>
+      <c r="M98" s="26"/>
+      <c r="N98" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O98" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="P98" s="30"/>
-      <c r="Q98" s="30"/>
-      <c r="R98" s="30"/>
+      <c r="P98" s="28"/>
+      <c r="Q98" s="28"/>
+      <c r="R98" s="28"/>
     </row>
     <row r="99" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="6" t="s">
@@ -3961,23 +3923,23 @@
       <c r="C99" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D99" s="37"/>
+      <c r="D99" s="35"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="31"/>
-      <c r="I99" s="30"/>
-      <c r="J99" s="30"/>
-      <c r="K99" s="30"/>
-      <c r="L99" s="30"/>
-      <c r="M99" s="28"/>
-      <c r="N99" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O99" s="30" t="n">
+      <c r="G99" s="26"/>
+      <c r="H99" s="29"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
+      <c r="K99" s="28"/>
+      <c r="L99" s="28"/>
+      <c r="M99" s="26"/>
+      <c r="N99" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O99" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="P99" s="34"/>
+      <c r="P99" s="32"/>
       <c r="Q99" s="10" t="s">
         <v>16</v>
       </c>
@@ -3992,104 +3954,104 @@
       <c r="C100" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="D100" s="32"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="31"/>
-      <c r="I100" s="30"/>
-      <c r="J100" s="30"/>
-      <c r="K100" s="30"/>
-      <c r="L100" s="30"/>
-      <c r="M100" s="28"/>
-      <c r="N100" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O100" s="30" t="n">
+      <c r="D100" s="30"/>
+      <c r="E100" s="30"/>
+      <c r="F100" s="30"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="28"/>
+      <c r="J100" s="28"/>
+      <c r="K100" s="28"/>
+      <c r="L100" s="28"/>
+      <c r="M100" s="26"/>
+      <c r="N100" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O100" s="28" t="n">
         <v>31</v>
       </c>
-      <c r="P100" s="30"/>
+      <c r="P100" s="28"/>
       <c r="Q100" s="7"/>
       <c r="R100" s="7"/>
     </row>
     <row r="101" customFormat="false" ht="4.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
-      <c r="H101" s="28"/>
-      <c r="I101" s="28"/>
-      <c r="J101" s="28"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
-      <c r="M101" s="28"/>
-      <c r="N101" s="28"/>
-      <c r="O101" s="28"/>
-      <c r="P101" s="28"/>
-      <c r="Q101" s="28"/>
-      <c r="R101" s="28"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="26"/>
+      <c r="K101" s="26"/>
+      <c r="L101" s="26"/>
+      <c r="M101" s="26"/>
+      <c r="N101" s="26"/>
+      <c r="O101" s="26"/>
+      <c r="P101" s="26"/>
+      <c r="Q101" s="26"/>
+      <c r="R101" s="26"/>
     </row>
     <row r="102" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="1"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="25" t="s">
+      <c r="D102" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E102" s="26"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="28"/>
-      <c r="H102" s="29"/>
-      <c r="I102" s="26"/>
-      <c r="J102" s="25" t="s">
+      <c r="E102" s="24"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="26"/>
+      <c r="H102" s="27"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="K102" s="26"/>
-      <c r="L102" s="27"/>
-      <c r="M102" s="28"/>
-      <c r="N102" s="29"/>
-      <c r="O102" s="26"/>
-      <c r="P102" s="25" t="s">
+      <c r="K102" s="24"/>
+      <c r="L102" s="25"/>
+      <c r="M102" s="26"/>
+      <c r="N102" s="27"/>
+      <c r="O102" s="24"/>
+      <c r="P102" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Q102" s="26"/>
-      <c r="R102" s="27"/>
+      <c r="Q102" s="24"/>
+      <c r="R102" s="25"/>
     </row>
     <row r="103" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C103" s="7"/>
-      <c r="D103" s="30"/>
-      <c r="E103" s="30"/>
-      <c r="F103" s="30"/>
-      <c r="G103" s="28"/>
-      <c r="H103" s="31" t="s">
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I103" s="30"/>
-      <c r="J103" s="30" t="s">
+      <c r="I103" s="28"/>
+      <c r="J103" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K103" s="30" t="s">
+      <c r="K103" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="L103" s="30" t="s">
+      <c r="L103" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M103" s="28"/>
-      <c r="N103" s="31" t="s">
+      <c r="M103" s="26"/>
+      <c r="N103" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="O103" s="30"/>
-      <c r="P103" s="30" t="s">
+      <c r="O103" s="28"/>
+      <c r="P103" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Q103" s="30" t="s">
+      <c r="Q103" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="R103" s="30" t="s">
+      <c r="R103" s="28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4100,35 +4062,35 @@
       <c r="C104" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D104" s="34"/>
+      <c r="D104" s="32"/>
       <c r="E104" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G104" s="28"/>
-      <c r="H104" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I104" s="30" t="n">
+      <c r="G104" s="26"/>
+      <c r="H104" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="J104" s="35"/>
-      <c r="K104" s="35"/>
-      <c r="L104" s="32"/>
-      <c r="M104" s="28"/>
-      <c r="N104" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O104" s="30" t="n">
+      <c r="J104" s="33"/>
+      <c r="K104" s="33"/>
+      <c r="L104" s="30"/>
+      <c r="M104" s="26"/>
+      <c r="N104" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O104" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="P104" s="38"/>
-      <c r="Q104" s="38" t="s">
+      <c r="P104" s="36"/>
+      <c r="Q104" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="R104" s="38"/>
+      <c r="R104" s="36"/>
     </row>
     <row r="105" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="6" t="s">
@@ -4137,31 +4099,31 @@
       <c r="C105" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D105" s="34"/>
+      <c r="D105" s="32"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I105" s="30" t="n">
+      <c r="G105" s="26"/>
+      <c r="H105" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I105" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="J105" s="32"/>
-      <c r="K105" s="32"/>
-      <c r="L105" s="32"/>
-      <c r="M105" s="28"/>
-      <c r="N105" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O105" s="30" t="n">
+      <c r="J105" s="30"/>
+      <c r="K105" s="30"/>
+      <c r="L105" s="30"/>
+      <c r="M105" s="26"/>
+      <c r="N105" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O105" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="P105" s="39"/>
-      <c r="Q105" s="40" t="s">
+      <c r="P105" s="37"/>
+      <c r="Q105" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="R105" s="40"/>
+      <c r="R105" s="38"/>
     </row>
     <row r="106" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="6" t="s">
@@ -4170,31 +4132,31 @@
       <c r="C106" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D106" s="35"/>
-      <c r="E106" s="32"/>
-      <c r="F106" s="32"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I106" s="30" t="n">
+      <c r="D106" s="33"/>
+      <c r="E106" s="30"/>
+      <c r="F106" s="30"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="J106" s="30"/>
-      <c r="K106" s="30"/>
-      <c r="L106" s="30"/>
-      <c r="M106" s="28"/>
-      <c r="N106" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O106" s="30" t="n">
+      <c r="J106" s="28"/>
+      <c r="K106" s="28"/>
+      <c r="L106" s="28"/>
+      <c r="M106" s="26"/>
+      <c r="N106" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O106" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="P106" s="38"/>
-      <c r="Q106" s="38" t="s">
+      <c r="P106" s="36"/>
+      <c r="Q106" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="R106" s="38"/>
+      <c r="R106" s="36"/>
     </row>
     <row r="107" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="6" t="s">
@@ -4203,35 +4165,35 @@
       <c r="C107" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D107" s="35"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="28"/>
-      <c r="H107" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I107" s="30" t="n">
+      <c r="D107" s="33"/>
+      <c r="E107" s="30"/>
+      <c r="F107" s="30"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I107" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="J107" s="30"/>
-      <c r="K107" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L107" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M107" s="28"/>
-      <c r="N107" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O107" s="30" t="n">
+      <c r="J107" s="28"/>
+      <c r="K107" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L107" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M107" s="26"/>
+      <c r="N107" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O107" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="P107" s="38"/>
-      <c r="Q107" s="40" t="s">
+      <c r="P107" s="36"/>
+      <c r="Q107" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="R107" s="40"/>
+      <c r="R107" s="38"/>
     </row>
     <row r="108" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="6" t="s">
@@ -4240,33 +4202,33 @@
       <c r="C108" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D108" s="35"/>
-      <c r="E108" s="32" t="s">
+      <c r="D108" s="33"/>
+      <c r="E108" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F108" s="32"/>
-      <c r="G108" s="28"/>
-      <c r="H108" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I108" s="30" t="n">
+      <c r="F108" s="30"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I108" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="J108" s="30"/>
+      <c r="J108" s="28"/>
       <c r="K108" s="7"/>
       <c r="L108" s="7"/>
-      <c r="M108" s="28"/>
-      <c r="N108" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O108" s="30" t="n">
+      <c r="M108" s="26"/>
+      <c r="N108" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O108" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="P108" s="38"/>
-      <c r="Q108" s="38" t="s">
+      <c r="P108" s="36"/>
+      <c r="Q108" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="R108" s="38"/>
+      <c r="R108" s="36"/>
     </row>
     <row r="109" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="6" t="s">
@@ -4275,35 +4237,35 @@
       <c r="C109" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="D109" s="32"/>
-      <c r="E109" s="32" t="s">
+      <c r="D109" s="30"/>
+      <c r="E109" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F109" s="32"/>
-      <c r="G109" s="28"/>
-      <c r="H109" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I109" s="30" t="n">
+      <c r="F109" s="30"/>
+      <c r="G109" s="26"/>
+      <c r="H109" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I109" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="J109" s="30"/>
-      <c r="K109" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L109" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M109" s="28"/>
-      <c r="N109" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O109" s="30" t="n">
+      <c r="J109" s="28"/>
+      <c r="K109" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L109" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M109" s="26"/>
+      <c r="N109" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O109" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="P109" s="32"/>
-      <c r="Q109" s="32"/>
-      <c r="R109" s="32"/>
+      <c r="P109" s="30"/>
+      <c r="Q109" s="30"/>
+      <c r="R109" s="30"/>
     </row>
     <row r="110" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="6" t="s">
@@ -4312,31 +4274,31 @@
       <c r="C110" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="D110" s="35"/>
-      <c r="E110" s="32" t="s">
+      <c r="D110" s="33"/>
+      <c r="E110" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F110" s="32"/>
-      <c r="G110" s="28"/>
-      <c r="H110" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I110" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="J110" s="30"/>
+      <c r="F110" s="30"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I110" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="J110" s="28"/>
       <c r="K110" s="7"/>
       <c r="L110" s="7"/>
-      <c r="M110" s="28"/>
-      <c r="N110" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O110" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="P110" s="30"/>
-      <c r="Q110" s="30"/>
-      <c r="R110" s="30"/>
+      <c r="M110" s="26"/>
+      <c r="N110" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O110" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="P110" s="28"/>
+      <c r="Q110" s="28"/>
+      <c r="R110" s="28"/>
     </row>
     <row r="111" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="6" t="s">
@@ -4345,33 +4307,33 @@
       <c r="C111" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="D111" s="32"/>
-      <c r="E111" s="32" t="s">
+      <c r="D111" s="30"/>
+      <c r="E111" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F111" s="32"/>
-      <c r="G111" s="28"/>
-      <c r="H111" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I111" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="J111" s="32"/>
-      <c r="K111" s="32"/>
-      <c r="L111" s="32"/>
-      <c r="M111" s="28"/>
-      <c r="N111" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O111" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="P111" s="30"/>
-      <c r="Q111" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R111" s="13" t="s">
+      <c r="F111" s="30"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="J111" s="30"/>
+      <c r="K111" s="30"/>
+      <c r="L111" s="30"/>
+      <c r="M111" s="26"/>
+      <c r="N111" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O111" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="P111" s="28"/>
+      <c r="Q111" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R111" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4382,29 +4344,29 @@
       <c r="C112" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="D112" s="32"/>
-      <c r="E112" s="32" t="s">
+      <c r="D112" s="30"/>
+      <c r="E112" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F112" s="32"/>
-      <c r="G112" s="28"/>
-      <c r="H112" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I112" s="30" t="n">
-        <v>9</v>
-      </c>
-      <c r="J112" s="32"/>
-      <c r="K112" s="32"/>
-      <c r="L112" s="32"/>
-      <c r="M112" s="28"/>
-      <c r="N112" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O112" s="30" t="n">
-        <v>9</v>
-      </c>
-      <c r="P112" s="30"/>
+      <c r="F112" s="30"/>
+      <c r="G112" s="26"/>
+      <c r="H112" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I112" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="J112" s="30"/>
+      <c r="K112" s="30"/>
+      <c r="L112" s="30"/>
+      <c r="M112" s="26"/>
+      <c r="N112" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O112" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="P112" s="28"/>
       <c r="Q112" s="7"/>
       <c r="R112" s="7"/>
     </row>
@@ -4415,31 +4377,31 @@
       <c r="C113" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="D113" s="32"/>
-      <c r="E113" s="32"/>
-      <c r="F113" s="32"/>
-      <c r="G113" s="28"/>
-      <c r="H113" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I113" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="J113" s="30"/>
-      <c r="K113" s="30"/>
-      <c r="L113" s="30"/>
-      <c r="M113" s="28"/>
-      <c r="N113" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O113" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="P113" s="34"/>
-      <c r="Q113" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R113" s="13" t="s">
+      <c r="D113" s="30"/>
+      <c r="E113" s="30"/>
+      <c r="F113" s="30"/>
+      <c r="G113" s="26"/>
+      <c r="H113" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I113" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="J113" s="28"/>
+      <c r="K113" s="28"/>
+      <c r="L113" s="28"/>
+      <c r="M113" s="26"/>
+      <c r="N113" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O113" s="28" t="n">
+        <v>10</v>
+      </c>
+      <c r="P113" s="32"/>
+      <c r="Q113" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R113" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4450,27 +4412,27 @@
       <c r="C114" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="D114" s="32"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="32"/>
-      <c r="G114" s="28"/>
-      <c r="H114" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I114" s="30" t="n">
-        <v>11</v>
-      </c>
-      <c r="J114" s="30"/>
-      <c r="K114" s="30"/>
-      <c r="L114" s="30"/>
-      <c r="M114" s="28"/>
-      <c r="N114" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O114" s="30" t="n">
-        <v>11</v>
-      </c>
-      <c r="P114" s="30"/>
+      <c r="D114" s="30"/>
+      <c r="E114" s="30"/>
+      <c r="F114" s="30"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I114" s="28" t="n">
+        <v>11</v>
+      </c>
+      <c r="J114" s="28"/>
+      <c r="K114" s="28"/>
+      <c r="L114" s="28"/>
+      <c r="M114" s="26"/>
+      <c r="N114" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O114" s="28" t="n">
+        <v>11</v>
+      </c>
+      <c r="P114" s="28"/>
       <c r="Q114" s="7"/>
       <c r="R114" s="7"/>
     </row>
@@ -4481,31 +4443,31 @@
       <c r="C115" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="D115" s="32"/>
-      <c r="E115" s="32" t="s">
+      <c r="D115" s="30"/>
+      <c r="E115" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F115" s="32"/>
-      <c r="G115" s="28"/>
-      <c r="H115" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I115" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="J115" s="30"/>
+      <c r="F115" s="30"/>
+      <c r="G115" s="26"/>
+      <c r="H115" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I115" s="28" t="n">
+        <v>12</v>
+      </c>
+      <c r="J115" s="28"/>
       <c r="K115" s="7"/>
       <c r="L115" s="7"/>
-      <c r="M115" s="28"/>
-      <c r="N115" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O115" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="P115" s="32"/>
-      <c r="Q115" s="32"/>
-      <c r="R115" s="32"/>
+      <c r="M115" s="26"/>
+      <c r="N115" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O115" s="28" t="n">
+        <v>12</v>
+      </c>
+      <c r="P115" s="30"/>
+      <c r="Q115" s="30"/>
+      <c r="R115" s="30"/>
     </row>
     <row r="116" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="6" t="s">
@@ -4514,33 +4476,33 @@
       <c r="C116" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="D116" s="35"/>
-      <c r="E116" s="32" t="s">
+      <c r="D116" s="33"/>
+      <c r="E116" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F116" s="32"/>
-      <c r="G116" s="28"/>
-      <c r="H116" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I116" s="30" t="n">
-        <v>13</v>
-      </c>
-      <c r="J116" s="41" t="s">
+      <c r="F116" s="30"/>
+      <c r="G116" s="26"/>
+      <c r="H116" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I116" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="J116" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="K116" s="41"/>
-      <c r="L116" s="41"/>
-      <c r="M116" s="28"/>
-      <c r="N116" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O116" s="30" t="n">
-        <v>13</v>
-      </c>
-      <c r="P116" s="32"/>
-      <c r="Q116" s="32"/>
-      <c r="R116" s="32"/>
+      <c r="K116" s="39"/>
+      <c r="L116" s="39"/>
+      <c r="M116" s="26"/>
+      <c r="N116" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O116" s="28" t="n">
+        <v>13</v>
+      </c>
+      <c r="P116" s="30"/>
+      <c r="Q116" s="30"/>
+      <c r="R116" s="30"/>
     </row>
     <row r="117" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="6" t="s">
@@ -4549,33 +4511,33 @@
       <c r="C117" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="D117" s="35"/>
-      <c r="E117" s="32" t="s">
+      <c r="D117" s="33"/>
+      <c r="E117" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F117" s="32"/>
-      <c r="G117" s="28"/>
-      <c r="H117" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I117" s="30" t="n">
+      <c r="F117" s="30"/>
+      <c r="G117" s="26"/>
+      <c r="H117" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I117" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="J117" s="41" t="s">
+      <c r="J117" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="K117" s="42"/>
-      <c r="L117" s="42"/>
-      <c r="M117" s="28"/>
-      <c r="N117" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O117" s="30" t="n">
+      <c r="K117" s="40"/>
+      <c r="L117" s="40"/>
+      <c r="M117" s="26"/>
+      <c r="N117" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O117" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="P117" s="30"/>
-      <c r="Q117" s="34"/>
-      <c r="R117" s="30"/>
+      <c r="P117" s="28"/>
+      <c r="Q117" s="32"/>
+      <c r="R117" s="28"/>
     </row>
     <row r="118" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="6" t="s">
@@ -4584,33 +4546,33 @@
       <c r="C118" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="D118" s="32"/>
-      <c r="E118" s="32" t="s">
+      <c r="D118" s="30"/>
+      <c r="E118" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F118" s="32"/>
-      <c r="G118" s="28"/>
-      <c r="H118" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I118" s="30" t="n">
+      <c r="F118" s="30"/>
+      <c r="G118" s="26"/>
+      <c r="H118" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="J118" s="32"/>
-      <c r="K118" s="32"/>
-      <c r="L118" s="32"/>
-      <c r="M118" s="28"/>
-      <c r="N118" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O118" s="30" t="n">
+      <c r="J118" s="30"/>
+      <c r="K118" s="30"/>
+      <c r="L118" s="30"/>
+      <c r="M118" s="26"/>
+      <c r="N118" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O118" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="P118" s="34"/>
-      <c r="Q118" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R118" s="13" t="s">
+      <c r="P118" s="32"/>
+      <c r="Q118" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R118" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4621,29 +4583,29 @@
       <c r="C119" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="D119" s="32"/>
-      <c r="E119" s="32" t="s">
+      <c r="D119" s="30"/>
+      <c r="E119" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F119" s="32"/>
-      <c r="G119" s="28"/>
-      <c r="H119" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I119" s="30" t="n">
-        <v>16</v>
-      </c>
-      <c r="J119" s="32"/>
-      <c r="K119" s="32"/>
-      <c r="L119" s="32"/>
-      <c r="M119" s="28"/>
-      <c r="N119" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O119" s="30" t="n">
-        <v>16</v>
-      </c>
-      <c r="P119" s="34"/>
+      <c r="F119" s="30"/>
+      <c r="G119" s="26"/>
+      <c r="H119" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I119" s="28" t="n">
+        <v>16</v>
+      </c>
+      <c r="J119" s="30"/>
+      <c r="K119" s="30"/>
+      <c r="L119" s="30"/>
+      <c r="M119" s="26"/>
+      <c r="N119" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O119" s="28" t="n">
+        <v>16</v>
+      </c>
+      <c r="P119" s="32"/>
       <c r="Q119" s="7"/>
       <c r="R119" s="7"/>
     </row>
@@ -4654,31 +4616,31 @@
       <c r="C120" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="D120" s="32"/>
-      <c r="E120" s="32"/>
-      <c r="F120" s="32"/>
-      <c r="G120" s="28"/>
-      <c r="H120" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I120" s="30" t="n">
-        <v>17</v>
-      </c>
-      <c r="J120" s="34"/>
-      <c r="K120" s="30"/>
-      <c r="L120" s="30"/>
-      <c r="M120" s="28"/>
-      <c r="N120" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O120" s="30" t="n">
-        <v>17</v>
-      </c>
-      <c r="P120" s="34"/>
-      <c r="Q120" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="R120" s="13" t="s">
+      <c r="D120" s="30"/>
+      <c r="E120" s="30"/>
+      <c r="F120" s="30"/>
+      <c r="G120" s="26"/>
+      <c r="H120" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I120" s="28" t="n">
+        <v>17</v>
+      </c>
+      <c r="J120" s="32"/>
+      <c r="K120" s="28"/>
+      <c r="L120" s="28"/>
+      <c r="M120" s="26"/>
+      <c r="N120" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O120" s="28" t="n">
+        <v>17</v>
+      </c>
+      <c r="P120" s="32"/>
+      <c r="Q120" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R120" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4689,31 +4651,31 @@
       <c r="C121" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D121" s="32"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32"/>
-      <c r="G121" s="28"/>
-      <c r="H121" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I121" s="30" t="n">
+      <c r="D121" s="30"/>
+      <c r="E121" s="30"/>
+      <c r="F121" s="30"/>
+      <c r="G121" s="26"/>
+      <c r="H121" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I121" s="28" t="n">
         <v>18</v>
       </c>
-      <c r="J121" s="34"/>
-      <c r="K121" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L121" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M121" s="28"/>
-      <c r="N121" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O121" s="30" t="n">
+      <c r="J121" s="32"/>
+      <c r="K121" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L121" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M121" s="26"/>
+      <c r="N121" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O121" s="28" t="n">
         <v>18</v>
       </c>
-      <c r="P121" s="30"/>
+      <c r="P121" s="28"/>
       <c r="Q121" s="7"/>
       <c r="R121" s="7"/>
     </row>
@@ -4724,29 +4686,29 @@
       <c r="C122" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="D122" s="30"/>
-      <c r="E122" s="30"/>
-      <c r="F122" s="30"/>
-      <c r="G122" s="28"/>
-      <c r="H122" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I122" s="30" t="n">
+      <c r="D122" s="28"/>
+      <c r="E122" s="28"/>
+      <c r="F122" s="28"/>
+      <c r="G122" s="26"/>
+      <c r="H122" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I122" s="28" t="n">
         <v>19</v>
       </c>
-      <c r="J122" s="34"/>
+      <c r="J122" s="32"/>
       <c r="K122" s="7"/>
       <c r="L122" s="7"/>
-      <c r="M122" s="28"/>
-      <c r="N122" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O122" s="30" t="n">
+      <c r="M122" s="26"/>
+      <c r="N122" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O122" s="28" t="n">
         <v>19</v>
       </c>
-      <c r="P122" s="32"/>
-      <c r="Q122" s="32"/>
-      <c r="R122" s="32"/>
+      <c r="P122" s="30"/>
+      <c r="Q122" s="30"/>
+      <c r="R122" s="30"/>
     </row>
     <row r="123" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="6" t="s">
@@ -4755,37 +4717,37 @@
       <c r="C123" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="D123" s="43"/>
-      <c r="E123" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F123" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G123" s="28"/>
-      <c r="H123" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I123" s="30" t="n">
+      <c r="D123" s="41"/>
+      <c r="E123" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G123" s="26"/>
+      <c r="H123" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I123" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="J123" s="30"/>
-      <c r="K123" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L123" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M123" s="28"/>
-      <c r="N123" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O123" s="30" t="n">
+      <c r="J123" s="28"/>
+      <c r="K123" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L123" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M123" s="26"/>
+      <c r="N123" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O123" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="P123" s="32"/>
-      <c r="Q123" s="32"/>
-      <c r="R123" s="32"/>
+      <c r="P123" s="30"/>
+      <c r="Q123" s="30"/>
+      <c r="R123" s="30"/>
     </row>
     <row r="124" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="6" t="s">
@@ -4794,29 +4756,29 @@
       <c r="C124" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="D124" s="30"/>
+      <c r="D124" s="28"/>
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
-      <c r="G124" s="28"/>
-      <c r="H124" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I124" s="30" t="n">
+      <c r="G124" s="26"/>
+      <c r="H124" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I124" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="J124" s="30"/>
-      <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
-      <c r="M124" s="28"/>
-      <c r="N124" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O124" s="30" t="n">
+      <c r="J124" s="28"/>
+      <c r="K124" s="28"/>
+      <c r="L124" s="28"/>
+      <c r="M124" s="26"/>
+      <c r="N124" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O124" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="P124" s="30"/>
-      <c r="Q124" s="30"/>
-      <c r="R124" s="30"/>
+      <c r="P124" s="28"/>
+      <c r="Q124" s="28"/>
+      <c r="R124" s="28"/>
     </row>
     <row r="125" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="6" t="s">
@@ -4825,35 +4787,35 @@
       <c r="C125" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="D125" s="34"/>
-      <c r="E125" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F125" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G125" s="28"/>
-      <c r="H125" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I125" s="30" t="n">
+      <c r="D125" s="32"/>
+      <c r="E125" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G125" s="26"/>
+      <c r="H125" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I125" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="J125" s="44"/>
-      <c r="K125" s="38" t="s">
+      <c r="J125" s="42"/>
+      <c r="K125" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L125" s="44" t="s">
+      <c r="L125" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="M125" s="28"/>
-      <c r="N125" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O125" s="30" t="n">
+      <c r="M125" s="26"/>
+      <c r="N125" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O125" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="P125" s="30"/>
+      <c r="P125" s="28"/>
       <c r="Q125" s="10" t="s">
         <v>16</v>
       </c>
@@ -4868,31 +4830,31 @@
       <c r="C126" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="D126" s="30"/>
+      <c r="D126" s="28"/>
       <c r="E126" s="7"/>
       <c r="F126" s="7"/>
-      <c r="G126" s="28"/>
-      <c r="H126" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I126" s="30" t="n">
+      <c r="G126" s="26"/>
+      <c r="H126" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I126" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="J126" s="32"/>
-      <c r="K126" s="38" t="s">
+      <c r="J126" s="30"/>
+      <c r="K126" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L126" s="32" t="s">
+      <c r="L126" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M126" s="28"/>
-      <c r="N126" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O126" s="30" t="n">
+      <c r="M126" s="26"/>
+      <c r="N126" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O126" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="P126" s="30"/>
+      <c r="P126" s="28"/>
       <c r="Q126" s="7"/>
       <c r="R126" s="7"/>
     </row>
@@ -4903,33 +4865,33 @@
       <c r="C127" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="D127" s="32"/>
-      <c r="E127" s="32"/>
-      <c r="F127" s="32"/>
-      <c r="G127" s="28"/>
-      <c r="H127" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I127" s="30" t="n">
+      <c r="D127" s="30"/>
+      <c r="E127" s="30"/>
+      <c r="F127" s="30"/>
+      <c r="G127" s="26"/>
+      <c r="H127" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I127" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="J127" s="41" t="s">
+      <c r="J127" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="K127" s="38" t="s">
+      <c r="K127" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L127" s="41" t="s">
+      <c r="L127" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="M127" s="28"/>
-      <c r="N127" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="O127" s="30" t="n">
+      <c r="M127" s="26"/>
+      <c r="N127" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O127" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="P127" s="30"/>
+      <c r="P127" s="28"/>
       <c r="Q127" s="10" t="s">
         <v>16</v>
       </c>
@@ -4944,31 +4906,31 @@
       <c r="C128" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="D128" s="32"/>
-      <c r="E128" s="32"/>
-      <c r="F128" s="32"/>
-      <c r="G128" s="28"/>
-      <c r="H128" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="I128" s="30" t="n">
+      <c r="D128" s="30"/>
+      <c r="E128" s="30"/>
+      <c r="F128" s="30"/>
+      <c r="G128" s="26"/>
+      <c r="H128" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I128" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="J128" s="38"/>
-      <c r="K128" s="38" t="s">
+      <c r="J128" s="36"/>
+      <c r="K128" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L128" s="38" t="s">
+      <c r="L128" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M128" s="28"/>
-      <c r="N128" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O128" s="30" t="n">
+      <c r="M128" s="26"/>
+      <c r="N128" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="O128" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="P128" s="45"/>
+      <c r="P128" s="43"/>
       <c r="Q128" s="7"/>
       <c r="R128" s="7"/>
     </row>
@@ -4979,33 +4941,33 @@
       <c r="C129" s="7" t="n">
         <v>26</v>
       </c>
-      <c r="D129" s="30"/>
-      <c r="E129" s="30"/>
-      <c r="F129" s="30"/>
-      <c r="G129" s="28"/>
-      <c r="H129" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I129" s="30" t="n">
+      <c r="D129" s="28"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="28"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I129" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="J129" s="38"/>
-      <c r="K129" s="38" t="s">
+      <c r="J129" s="36"/>
+      <c r="K129" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L129" s="38" t="s">
+      <c r="L129" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M129" s="28"/>
-      <c r="N129" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="O129" s="30" t="n">
+      <c r="M129" s="26"/>
+      <c r="N129" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O129" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="P129" s="32"/>
-      <c r="Q129" s="32"/>
-      <c r="R129" s="32"/>
+      <c r="P129" s="30"/>
+      <c r="Q129" s="30"/>
+      <c r="R129" s="30"/>
     </row>
     <row r="130" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="6" t="s">
@@ -5014,37 +4976,37 @@
       <c r="C130" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="D130" s="30"/>
+      <c r="D130" s="28"/>
       <c r="E130" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F130" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G130" s="28"/>
-      <c r="H130" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I130" s="30" t="n">
+      <c r="G130" s="26"/>
+      <c r="H130" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I130" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="J130" s="38"/>
-      <c r="K130" s="38" t="s">
+      <c r="J130" s="36"/>
+      <c r="K130" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L130" s="38" t="s">
+      <c r="L130" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M130" s="28"/>
-      <c r="N130" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O130" s="30" t="n">
+      <c r="M130" s="26"/>
+      <c r="N130" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O130" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="P130" s="35"/>
-      <c r="Q130" s="32"/>
-      <c r="R130" s="32"/>
+      <c r="P130" s="33"/>
+      <c r="Q130" s="30"/>
+      <c r="R130" s="30"/>
     </row>
     <row r="131" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="6" t="s">
@@ -5053,33 +5015,33 @@
       <c r="C131" s="7" t="n">
         <v>28</v>
       </c>
-      <c r="D131" s="30"/>
+      <c r="D131" s="28"/>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
-      <c r="G131" s="28"/>
-      <c r="H131" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I131" s="30" t="n">
+      <c r="G131" s="26"/>
+      <c r="H131" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I131" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="J131" s="38"/>
-      <c r="K131" s="38" t="s">
+      <c r="J131" s="36"/>
+      <c r="K131" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L131" s="38" t="s">
+      <c r="L131" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M131" s="28"/>
-      <c r="N131" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O131" s="30" t="n">
+      <c r="M131" s="26"/>
+      <c r="N131" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O131" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="P131" s="30"/>
-      <c r="Q131" s="30"/>
-      <c r="R131" s="30"/>
+      <c r="P131" s="28"/>
+      <c r="Q131" s="28"/>
+      <c r="R131" s="28"/>
     </row>
     <row r="132" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="6" t="s">
@@ -5088,37 +5050,37 @@
       <c r="C132" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="D132" s="34"/>
+      <c r="D132" s="32"/>
       <c r="E132" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F132" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G132" s="28"/>
-      <c r="H132" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="I132" s="30" t="n">
+      <c r="G132" s="26"/>
+      <c r="H132" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="J132" s="32"/>
-      <c r="K132" s="38" t="s">
+      <c r="J132" s="30"/>
+      <c r="K132" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L132" s="32" t="s">
+      <c r="L132" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M132" s="28"/>
-      <c r="N132" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="O132" s="30" t="n">
+      <c r="M132" s="26"/>
+      <c r="N132" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="O132" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="P132" s="30"/>
-      <c r="Q132" s="30"/>
-      <c r="R132" s="30"/>
+      <c r="P132" s="28"/>
+      <c r="Q132" s="28"/>
+      <c r="R132" s="28"/>
     </row>
     <row r="133" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="6" t="s">
@@ -5127,58 +5089,58 @@
       <c r="C133" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D133" s="30"/>
+      <c r="D133" s="28"/>
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
-      <c r="G133" s="28"/>
-      <c r="H133" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I133" s="30" t="n">
+      <c r="G133" s="26"/>
+      <c r="H133" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I133" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="J133" s="35"/>
-      <c r="K133" s="38" t="s">
+      <c r="J133" s="33"/>
+      <c r="K133" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L133" s="32" t="s">
+      <c r="L133" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M133" s="28"/>
-      <c r="N133" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="O133" s="30" t="n">
+      <c r="M133" s="26"/>
+      <c r="N133" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="O133" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="P133" s="30"/>
-      <c r="Q133" s="30"/>
-      <c r="R133" s="30"/>
+      <c r="P133" s="28"/>
+      <c r="Q133" s="28"/>
+      <c r="R133" s="28"/>
     </row>
     <row r="134" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="6"/>
       <c r="C134" s="7"/>
-      <c r="D134" s="30"/>
-      <c r="E134" s="30"/>
-      <c r="F134" s="30"/>
-      <c r="G134" s="46"/>
-      <c r="H134" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I134" s="30" t="n">
+      <c r="D134" s="28"/>
+      <c r="E134" s="28"/>
+      <c r="F134" s="28"/>
+      <c r="G134" s="44"/>
+      <c r="H134" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I134" s="28" t="n">
         <v>31</v>
       </c>
-      <c r="J134" s="47"/>
-      <c r="K134" s="38" t="s">
+      <c r="J134" s="45"/>
+      <c r="K134" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="L134" s="38"/>
-      <c r="M134" s="46"/>
-      <c r="N134" s="31"/>
-      <c r="O134" s="30"/>
-      <c r="P134" s="30"/>
-      <c r="Q134" s="30"/>
-      <c r="R134" s="30"/>
+      <c r="L134" s="36"/>
+      <c r="M134" s="44"/>
+      <c r="N134" s="29"/>
+      <c r="O134" s="28"/>
+      <c r="P134" s="28"/>
+      <c r="Q134" s="28"/>
+      <c r="R134" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
aanpassing agenda + stages volzet
</commit_message>
<xml_diff>
--- a/flyers/Mechelen_2020-21.xlsx
+++ b/flyers/Mechelen_2020-21.xlsx
@@ -574,11 +574,11 @@
   </sheetPr>
   <dimension ref="B1:R134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="L12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="2.83"/>
@@ -2115,11 +2115,11 @@
         <v>10</v>
       </c>
       <c r="J46" s="7"/>
-      <c r="K46" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>17</v>
+      <c r="K46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="M46" s="8"/>
       <c r="N46" s="6" t="s">
@@ -2185,11 +2185,11 @@
         <v>12</v>
       </c>
       <c r="J48" s="7"/>
-      <c r="K48" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L48" s="11" t="s">
-        <v>17</v>
+      <c r="K48" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L48" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="M48" s="8"/>
       <c r="N48" s="6" t="s">
@@ -2694,11 +2694,11 @@
         <v>27</v>
       </c>
       <c r="D63" s="7"/>
-      <c r="E63" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>16</v>
+      <c r="E63" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="G63" s="8"/>
       <c r="H63" s="6" t="s">
@@ -2762,11 +2762,11 @@
         <v>29</v>
       </c>
       <c r="D65" s="7"/>
-      <c r="E65" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>16</v>
+      <c r="E65" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="G65" s="8"/>
       <c r="H65" s="6" t="s">

</xml_diff>